<commit_message>
Excel To CSV 工具修改
</commit_message>
<xml_diff>
--- a/ExcelToJs/excel_data/Goods.xlsx
+++ b/ExcelToJs/excel_data/Goods.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="China" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>物品描述1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -113,73 +113,108 @@
     <t>英国物品9</t>
   </si>
   <si>
-    <t>name.string</t>
-  </si>
-  <si>
-    <t>desc.string</t>
+    <t>price.float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>existenceTime.float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出生点1|出生点2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>id.int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>price.float</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>existenceTime.float</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出生点1|出生点2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>出生点9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出生点8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出生点6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10|12</t>
+  </si>
+  <si>
+    <t>10|13</t>
+  </si>
+  <si>
+    <t>10|14</t>
+  </si>
+  <si>
+    <t>10|15</t>
+  </si>
+  <si>
+    <t>10|16</t>
+  </si>
+  <si>
+    <t>10|17</t>
+  </si>
+  <si>
+    <t>10|18</t>
+  </si>
+  <si>
+    <t>10|19</t>
+  </si>
+  <si>
+    <t>物,品,描,述1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物,品,描,述2</t>
+  </si>
+  <si>
+    <t>物,品,描,述3</t>
+  </si>
+  <si>
+    <t>物,品,描,述4</t>
+  </si>
+  <si>
+    <t>物,品,描,述5</t>
+  </si>
+  <si>
+    <t>物,品,描,述6</t>
+  </si>
+  <si>
+    <t>物,品,描,述7</t>
+  </si>
+  <si>
+    <t>物,品,描,述8</t>
+  </si>
+  <si>
+    <t>物,品,描,述9</t>
   </si>
   <si>
     <t>id.int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>出生点9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出生点8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出生点6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bornPoint.string.array</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10|12</t>
-  </si>
-  <si>
-    <t>10|13</t>
-  </si>
-  <si>
-    <t>10|14</t>
-  </si>
-  <si>
-    <t>10|15</t>
-  </si>
-  <si>
-    <t>10|16</t>
-  </si>
-  <si>
-    <t>10|17</t>
-  </si>
-  <si>
-    <t>10|18</t>
-  </si>
-  <si>
-    <t>10|19</t>
-  </si>
-  <si>
-    <t>bornPoint.float.array</t>
+    <t>name.String</t>
+  </si>
+  <si>
+    <t>name.String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc.String</t>
+  </si>
+  <si>
+    <t>desc.String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bornPoint.String.array</t>
+  </si>
+  <si>
+    <t>bornPoint.float.array.aaa</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -531,13 +566,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.875" customWidth="1"/>
     <col min="2" max="3" width="13.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
@@ -546,22 +581,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -575,10 +610,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>10000</v>
+        <v>10000.999999899999</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F2">
         <v>30</v>
@@ -675,7 +710,7 @@
         <v>60000</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F7">
         <v>80</v>
@@ -715,7 +750,7 @@
         <v>80000</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -735,7 +770,7 @@
         <v>90000</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F10">
         <v>110</v>
@@ -752,34 +787,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -790,7 +828,7 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D2">
         <v>10000</v>
@@ -807,13 +845,13 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="D3">
         <v>20000</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F3">
         <v>40</v>
@@ -827,13 +865,13 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>30000</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F4">
         <v>50</v>
@@ -847,13 +885,13 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="D5">
         <v>40000</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F5">
         <v>60</v>
@@ -867,13 +905,13 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>50000</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F6">
         <v>70</v>
@@ -887,13 +925,13 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="D7">
         <v>60000</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F7">
         <v>80</v>
@@ -907,13 +945,13 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="D8">
         <v>70000</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F8">
         <v>90</v>
@@ -927,13 +965,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D9">
         <v>80000</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -947,13 +985,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="D10">
         <v>90000</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F10">
         <v>110</v>

</xml_diff>